<commit_message>
complete chord detection in actual songs
</commit_message>
<xml_diff>
--- a/Exp_data/Chord.xlsx
+++ b/Exp_data/Chord.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samdy\PycharmProjects\Bocchi_the_Chord\Exp_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7455E111-371B-4C58-AC64-41D82F2897CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D40CF840-A9DF-4B3D-A288-B0FD5FA10BA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="2408" windowWidth="18225" windowHeight="11872" xr2:uid="{C45753D4-B38A-4C27-ABED-523AECCA5630}"/>
+    <workbookView xWindow="5115" yWindow="2483" windowWidth="18225" windowHeight="11872" xr2:uid="{C45753D4-B38A-4C27-ABED-523AECCA5630}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -488,8 +488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A1C5292-AC85-4290-A9BF-11C99256D61C}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>